<commit_message>
updated javadoc + fhir IG
</commit_message>
<xml_diff>
--- a/docs/src/.vuepress/public/fhir/ImplementationGuide/dev.dsf/StructureDefinition-task.xlsx
+++ b/docs/src/.vuepress/public/fhir/ImplementationGuide/dev.dsf/StructureDefinition-task.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5551" uniqueCount="666">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5551" uniqueCount="667">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-27</t>
+    <t>2025-11-26</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -890,7 +890,7 @@
     <t>Task.requester</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://dsf.dev/fhir/StructureDefinition/organization|2.0.0)
+    <t xml:space="preserve">Reference(http://dsf.dev/fhir/StructureDefinition/organization|2.0.0|Practitioner)
 </t>
   </si>
   <si>
@@ -1458,6 +1458,10 @@
   </si>
   <si>
     <t>Task.restriction.recipient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(http://dsf.dev/fhir/StructureDefinition/organization|2.0.0)
+</t>
   </si>
   <si>
     <t>For whom is fulfillment sought?</t>
@@ -9064,13 +9068,13 @@
         <v>20</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>282</v>
+        <v>465</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" s="2"/>
@@ -9133,13 +9137,13 @@
         <v>20</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="AK59" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="AM59" t="s" s="2">
         <v>20</v>
@@ -9150,10 +9154,10 @@
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -9262,10 +9266,10 @@
     </row>
     <row r="61">
       <c r="A61" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -9376,10 +9380,10 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
@@ -9490,10 +9494,10 @@
     </row>
     <row r="63">
       <c r="A63" t="s" s="2">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -9604,10 +9608,10 @@
     </row>
     <row r="64">
       <c r="A64" t="s" s="2">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
@@ -9718,10 +9722,10 @@
     </row>
     <row r="65">
       <c r="A65" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
@@ -9830,10 +9834,10 @@
     </row>
     <row r="66">
       <c r="A66" t="s" s="2">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
@@ -9944,10 +9948,10 @@
     </row>
     <row r="67">
       <c r="A67" t="s" s="2">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s" s="2">
@@ -10060,10 +10064,10 @@
     </row>
     <row r="68">
       <c r="A68" t="s" s="2">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B68" t="s" s="2">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" t="s" s="2">
@@ -10176,10 +10180,10 @@
     </row>
     <row r="69">
       <c r="A69" t="s" s="2">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" t="s" s="2">
@@ -10221,7 +10225,7 @@
       </c>
       <c r="Q69" s="2"/>
       <c r="R69" t="s" s="2">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="S69" t="s" s="2">
         <v>20</v>
@@ -10292,10 +10296,10 @@
     </row>
     <row r="70">
       <c r="A70" t="s" s="2">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" t="s" s="2">
@@ -10406,10 +10410,10 @@
     </row>
     <row r="71">
       <c r="A71" t="s" s="2">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" t="s" s="2">
@@ -10518,10 +10522,10 @@
     </row>
     <row r="72">
       <c r="A72" t="s" s="2">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s" s="2">
@@ -10632,10 +10636,10 @@
     </row>
     <row r="73">
       <c r="A73" t="s" s="2">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" t="s" s="2">
@@ -10746,14 +10750,14 @@
     </row>
     <row r="74">
       <c r="A74" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s" s="2">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74" t="s" s="2">
@@ -10775,14 +10779,14 @@
         <v>440</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="M74" t="s" s="2">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="N74" s="2"/>
       <c r="O74" t="s" s="2">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="P74" t="s" s="2">
         <v>20</v>
@@ -10819,17 +10823,17 @@
         <v>20</v>
       </c>
       <c r="AB74" t="s" s="2">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="AC74" s="2"/>
       <c r="AD74" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AE74" t="s" s="2">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="AF74" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="AG74" t="s" s="2">
         <v>75</v>
@@ -10847,7 +10851,7 @@
         <v>20</v>
       </c>
       <c r="AL74" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="AM74" t="s" s="2">
         <v>20</v>
@@ -10858,10 +10862,10 @@
     </row>
     <row r="75">
       <c r="A75" t="s" s="2">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" t="s" s="2">
@@ -10970,10 +10974,10 @@
     </row>
     <row r="76">
       <c r="A76" t="s" s="2">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B76" t="s" s="2">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" t="s" s="2">
@@ -11084,10 +11088,10 @@
     </row>
     <row r="77">
       <c r="A77" t="s" s="2">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="B77" t="s" s="2">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" t="s" s="2">
@@ -11200,14 +11204,14 @@
     </row>
     <row r="78">
       <c r="A78" t="s" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B78" t="s" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" t="s" s="2">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="E78" s="2"/>
       <c r="F78" t="s" s="2">
@@ -11229,16 +11233,16 @@
         <v>189</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="M78" t="s" s="2">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="N78" t="s" s="2">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="O78" t="s" s="2">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="P78" t="s" s="2">
         <v>20</v>
@@ -11266,7 +11270,7 @@
         <v>193</v>
       </c>
       <c r="Y78" t="s" s="2">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="Z78" t="s" s="2">
         <v>20</v>
@@ -11287,7 +11291,7 @@
         <v>20</v>
       </c>
       <c r="AF78" t="s" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="AG78" t="s" s="2">
         <v>84</v>
@@ -11305,7 +11309,7 @@
         <v>20</v>
       </c>
       <c r="AL78" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="AM78" t="s" s="2">
         <v>20</v>
@@ -11316,10 +11320,10 @@
     </row>
     <row r="79">
       <c r="A79" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B79" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" t="s" s="2">
@@ -11342,13 +11346,13 @@
         <v>20</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="M79" t="s" s="2">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="N79" s="2"/>
       <c r="O79" s="2"/>
@@ -11399,7 +11403,7 @@
         <v>20</v>
       </c>
       <c r="AF79" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="AG79" t="s" s="2">
         <v>84</v>
@@ -11417,7 +11421,7 @@
         <v>20</v>
       </c>
       <c r="AL79" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="AM79" t="s" s="2">
         <v>20</v>
@@ -11428,16 +11432,16 @@
     </row>
     <row r="80">
       <c r="A80" t="s" s="2">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B80" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C80" t="s" s="2">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="D80" t="s" s="2">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80" t="s" s="2">
@@ -11459,14 +11463,14 @@
         <v>440</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="M80" t="s" s="2">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="N80" s="2"/>
       <c r="O80" t="s" s="2">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="P80" t="s" s="2">
         <v>20</v>
@@ -11515,7 +11519,7 @@
         <v>20</v>
       </c>
       <c r="AF80" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="AG80" t="s" s="2">
         <v>75</v>
@@ -11533,7 +11537,7 @@
         <v>20</v>
       </c>
       <c r="AL80" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="AM80" t="s" s="2">
         <v>20</v>
@@ -11544,10 +11548,10 @@
     </row>
     <row r="81">
       <c r="A81" t="s" s="2">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B81" t="s" s="2">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" t="s" s="2">
@@ -11656,10 +11660,10 @@
     </row>
     <row r="82">
       <c r="A82" t="s" s="2">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B82" t="s" s="2">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" t="s" s="2">
@@ -11770,10 +11774,10 @@
     </row>
     <row r="83">
       <c r="A83" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B83" t="s" s="2">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" t="s" s="2">
@@ -11886,14 +11890,14 @@
     </row>
     <row r="84">
       <c r="A84" t="s" s="2">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B84" t="s" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" t="s" s="2">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84" t="s" s="2">
@@ -11915,16 +11919,16 @@
         <v>189</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="M84" t="s" s="2">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="N84" t="s" s="2">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="O84" t="s" s="2">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="P84" t="s" s="2">
         <v>20</v>
@@ -11953,7 +11957,7 @@
       </c>
       <c r="Y84" s="2"/>
       <c r="Z84" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="AA84" t="s" s="2">
         <v>20</v>
@@ -11971,7 +11975,7 @@
         <v>20</v>
       </c>
       <c r="AF84" t="s" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="AG84" t="s" s="2">
         <v>84</v>
@@ -11989,7 +11993,7 @@
         <v>20</v>
       </c>
       <c r="AL84" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="AM84" t="s" s="2">
         <v>20</v>
@@ -12000,10 +12004,10 @@
     </row>
     <row r="85">
       <c r="A85" t="s" s="2">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B85" t="s" s="2">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" t="s" s="2">
@@ -12112,10 +12116,10 @@
     </row>
     <row r="86">
       <c r="A86" t="s" s="2">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B86" t="s" s="2">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" t="s" s="2">
@@ -12226,10 +12230,10 @@
     </row>
     <row r="87">
       <c r="A87" t="s" s="2">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B87" t="s" s="2">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" t="s" s="2">
@@ -12252,19 +12256,19 @@
         <v>85</v>
       </c>
       <c r="K87" t="s" s="2">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="L87" t="s" s="2">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="M87" t="s" s="2">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="N87" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="O87" t="s" s="2">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="P87" t="s" s="2">
         <v>20</v>
@@ -12313,7 +12317,7 @@
         <v>20</v>
       </c>
       <c r="AF87" t="s" s="2">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="AG87" t="s" s="2">
         <v>75</v>
@@ -12331,21 +12335,21 @@
         <v>20</v>
       </c>
       <c r="AL87" t="s" s="2">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="AM87" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN87" t="s" s="2">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s" s="2">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B88" t="s" s="2">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" t="s" s="2">
@@ -12454,10 +12458,10 @@
     </row>
     <row r="89">
       <c r="A89" t="s" s="2">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="B89" t="s" s="2">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" t="s" s="2">
@@ -12568,10 +12572,10 @@
     </row>
     <row r="90">
       <c r="A90" t="s" s="2">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B90" t="s" s="2">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" t="s" s="2">
@@ -12597,23 +12601,23 @@
         <v>98</v>
       </c>
       <c r="L90" t="s" s="2">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="M90" t="s" s="2">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="N90" t="s" s="2">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="O90" t="s" s="2">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="P90" t="s" s="2">
         <v>20</v>
       </c>
       <c r="Q90" s="2"/>
       <c r="R90" t="s" s="2">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="S90" t="s" s="2">
         <v>20</v>
@@ -12655,7 +12659,7 @@
         <v>20</v>
       </c>
       <c r="AF90" t="s" s="2">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="AG90" t="s" s="2">
         <v>75</v>
@@ -12673,21 +12677,21 @@
         <v>20</v>
       </c>
       <c r="AL90" t="s" s="2">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="AM90" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN90" t="s" s="2">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s" s="2">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B91" t="s" s="2">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" t="s" s="2">
@@ -12713,13 +12717,13 @@
         <v>232</v>
       </c>
       <c r="L91" t="s" s="2">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="M91" t="s" s="2">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N91" t="s" s="2">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="O91" s="2"/>
       <c r="P91" t="s" s="2">
@@ -12769,7 +12773,7 @@
         <v>20</v>
       </c>
       <c r="AF91" t="s" s="2">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="AG91" t="s" s="2">
         <v>75</v>
@@ -12787,21 +12791,21 @@
         <v>20</v>
       </c>
       <c r="AL91" t="s" s="2">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="AM91" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN91" t="s" s="2">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s" s="2">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B92" t="s" s="2">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" t="s" s="2">
@@ -12827,21 +12831,21 @@
         <v>104</v>
       </c>
       <c r="L92" t="s" s="2">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="M92" t="s" s="2">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="N92" s="2"/>
       <c r="O92" t="s" s="2">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="P92" t="s" s="2">
         <v>20</v>
       </c>
       <c r="Q92" s="2"/>
       <c r="R92" t="s" s="2">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="S92" t="s" s="2">
         <v>20</v>
@@ -12883,7 +12887,7 @@
         <v>20</v>
       </c>
       <c r="AF92" t="s" s="2">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="AG92" t="s" s="2">
         <v>75</v>
@@ -12901,21 +12905,21 @@
         <v>20</v>
       </c>
       <c r="AL92" t="s" s="2">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="AM92" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN92" t="s" s="2">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s" s="2">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B93" t="s" s="2">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" t="s" s="2">
@@ -12941,14 +12945,14 @@
         <v>232</v>
       </c>
       <c r="L93" t="s" s="2">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="M93" t="s" s="2">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="N93" s="2"/>
       <c r="O93" t="s" s="2">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="P93" t="s" s="2">
         <v>20</v>
@@ -12997,7 +13001,7 @@
         <v>20</v>
       </c>
       <c r="AF93" t="s" s="2">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="AG93" t="s" s="2">
         <v>75</v>
@@ -13015,21 +13019,21 @@
         <v>20</v>
       </c>
       <c r="AL93" t="s" s="2">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="AM93" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN93" t="s" s="2">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s" s="2">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B94" t="s" s="2">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" t="s" s="2">
@@ -13052,19 +13056,19 @@
         <v>85</v>
       </c>
       <c r="K94" t="s" s="2">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="L94" t="s" s="2">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="M94" t="s" s="2">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="N94" t="s" s="2">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="O94" t="s" s="2">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="P94" t="s" s="2">
         <v>20</v>
@@ -13113,7 +13117,7 @@
         <v>20</v>
       </c>
       <c r="AF94" t="s" s="2">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="AG94" t="s" s="2">
         <v>75</v>
@@ -13131,21 +13135,21 @@
         <v>20</v>
       </c>
       <c r="AL94" t="s" s="2">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="AM94" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN94" t="s" s="2">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s" s="2">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="B95" t="s" s="2">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" t="s" s="2">
@@ -13171,16 +13175,16 @@
         <v>232</v>
       </c>
       <c r="L95" t="s" s="2">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="M95" t="s" s="2">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="N95" t="s" s="2">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="O95" t="s" s="2">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="P95" t="s" s="2">
         <v>20</v>
@@ -13229,7 +13233,7 @@
         <v>20</v>
       </c>
       <c r="AF95" t="s" s="2">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="AG95" t="s" s="2">
         <v>75</v>
@@ -13247,21 +13251,21 @@
         <v>20</v>
       </c>
       <c r="AL95" t="s" s="2">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="AM95" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN95" t="s" s="2">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s" s="2">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B96" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" t="s" s="2">
@@ -13287,10 +13291,10 @@
         <v>232</v>
       </c>
       <c r="L96" t="s" s="2">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="M96" t="s" s="2">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="N96" s="2"/>
       <c r="O96" s="2"/>
@@ -13341,7 +13345,7 @@
         <v>20</v>
       </c>
       <c r="AF96" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="AG96" t="s" s="2">
         <v>84</v>
@@ -13359,7 +13363,7 @@
         <v>20</v>
       </c>
       <c r="AL96" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="AM96" t="s" s="2">
         <v>20</v>
@@ -13370,16 +13374,16 @@
     </row>
     <row r="97">
       <c r="A97" t="s" s="2">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B97" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C97" t="s" s="2">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="D97" t="s" s="2">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="E97" s="2"/>
       <c r="F97" t="s" s="2">
@@ -13401,14 +13405,14 @@
         <v>440</v>
       </c>
       <c r="L97" t="s" s="2">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="M97" t="s" s="2">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="N97" s="2"/>
       <c r="O97" t="s" s="2">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="P97" t="s" s="2">
         <v>20</v>
@@ -13457,7 +13461,7 @@
         <v>20</v>
       </c>
       <c r="AF97" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="AG97" t="s" s="2">
         <v>75</v>
@@ -13475,7 +13479,7 @@
         <v>20</v>
       </c>
       <c r="AL97" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="AM97" t="s" s="2">
         <v>20</v>
@@ -13486,10 +13490,10 @@
     </row>
     <row r="98">
       <c r="A98" t="s" s="2">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="B98" t="s" s="2">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" t="s" s="2">
@@ -13598,10 +13602,10 @@
     </row>
     <row r="99">
       <c r="A99" t="s" s="2">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="B99" t="s" s="2">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" t="s" s="2">
@@ -13712,10 +13716,10 @@
     </row>
     <row r="100">
       <c r="A100" t="s" s="2">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="B100" t="s" s="2">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" t="s" s="2">
@@ -13828,14 +13832,14 @@
     </row>
     <row r="101">
       <c r="A101" t="s" s="2">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="B101" t="s" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C101" s="2"/>
       <c r="D101" t="s" s="2">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="E101" s="2"/>
       <c r="F101" t="s" s="2">
@@ -13857,16 +13861,16 @@
         <v>189</v>
       </c>
       <c r="L101" t="s" s="2">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="M101" t="s" s="2">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="N101" t="s" s="2">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="O101" t="s" s="2">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="P101" t="s" s="2">
         <v>20</v>
@@ -13895,7 +13899,7 @@
       </c>
       <c r="Y101" s="2"/>
       <c r="Z101" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="AA101" t="s" s="2">
         <v>20</v>
@@ -13913,7 +13917,7 @@
         <v>20</v>
       </c>
       <c r="AF101" t="s" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="AG101" t="s" s="2">
         <v>84</v>
@@ -13931,7 +13935,7 @@
         <v>20</v>
       </c>
       <c r="AL101" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="AM101" t="s" s="2">
         <v>20</v>
@@ -13942,10 +13946,10 @@
     </row>
     <row r="102">
       <c r="A102" t="s" s="2">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="B102" t="s" s="2">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C102" s="2"/>
       <c r="D102" t="s" s="2">
@@ -14054,10 +14058,10 @@
     </row>
     <row r="103">
       <c r="A103" t="s" s="2">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="B103" t="s" s="2">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="C103" s="2"/>
       <c r="D103" t="s" s="2">
@@ -14168,10 +14172,10 @@
     </row>
     <row r="104">
       <c r="A104" t="s" s="2">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="B104" t="s" s="2">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C104" s="2"/>
       <c r="D104" t="s" s="2">
@@ -14194,19 +14198,19 @@
         <v>85</v>
       </c>
       <c r="K104" t="s" s="2">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="L104" t="s" s="2">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="M104" t="s" s="2">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="N104" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="O104" t="s" s="2">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="P104" t="s" s="2">
         <v>20</v>
@@ -14255,7 +14259,7 @@
         <v>20</v>
       </c>
       <c r="AF104" t="s" s="2">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="AG104" t="s" s="2">
         <v>75</v>
@@ -14273,21 +14277,21 @@
         <v>20</v>
       </c>
       <c r="AL104" t="s" s="2">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="AM104" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN104" t="s" s="2">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s" s="2">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="B105" t="s" s="2">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C105" s="2"/>
       <c r="D105" t="s" s="2">
@@ -14396,10 +14400,10 @@
     </row>
     <row r="106">
       <c r="A106" t="s" s="2">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="B106" t="s" s="2">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C106" s="2"/>
       <c r="D106" t="s" s="2">
@@ -14510,10 +14514,10 @@
     </row>
     <row r="107">
       <c r="A107" t="s" s="2">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="B107" t="s" s="2">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="C107" s="2"/>
       <c r="D107" t="s" s="2">
@@ -14539,23 +14543,23 @@
         <v>98</v>
       </c>
       <c r="L107" t="s" s="2">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="M107" t="s" s="2">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="N107" t="s" s="2">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="O107" t="s" s="2">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="P107" t="s" s="2">
         <v>20</v>
       </c>
       <c r="Q107" s="2"/>
       <c r="R107" t="s" s="2">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="S107" t="s" s="2">
         <v>20</v>
@@ -14597,7 +14601,7 @@
         <v>20</v>
       </c>
       <c r="AF107" t="s" s="2">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="AG107" t="s" s="2">
         <v>75</v>
@@ -14615,21 +14619,21 @@
         <v>20</v>
       </c>
       <c r="AL107" t="s" s="2">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="AM107" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN107" t="s" s="2">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s" s="2">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="B108" t="s" s="2">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="C108" s="2"/>
       <c r="D108" t="s" s="2">
@@ -14655,13 +14659,13 @@
         <v>232</v>
       </c>
       <c r="L108" t="s" s="2">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="M108" t="s" s="2">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N108" t="s" s="2">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="O108" s="2"/>
       <c r="P108" t="s" s="2">
@@ -14711,7 +14715,7 @@
         <v>20</v>
       </c>
       <c r="AF108" t="s" s="2">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="AG108" t="s" s="2">
         <v>75</v>
@@ -14729,21 +14733,21 @@
         <v>20</v>
       </c>
       <c r="AL108" t="s" s="2">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="AM108" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN108" t="s" s="2">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s" s="2">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="B109" t="s" s="2">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C109" s="2"/>
       <c r="D109" t="s" s="2">
@@ -14769,21 +14773,21 @@
         <v>104</v>
       </c>
       <c r="L109" t="s" s="2">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="M109" t="s" s="2">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="N109" s="2"/>
       <c r="O109" t="s" s="2">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="P109" t="s" s="2">
         <v>20</v>
       </c>
       <c r="Q109" s="2"/>
       <c r="R109" t="s" s="2">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="S109" t="s" s="2">
         <v>20</v>
@@ -14825,7 +14829,7 @@
         <v>20</v>
       </c>
       <c r="AF109" t="s" s="2">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="AG109" t="s" s="2">
         <v>75</v>
@@ -14843,21 +14847,21 @@
         <v>20</v>
       </c>
       <c r="AL109" t="s" s="2">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="AM109" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN109" t="s" s="2">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s" s="2">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B110" t="s" s="2">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C110" s="2"/>
       <c r="D110" t="s" s="2">
@@ -14883,14 +14887,14 @@
         <v>232</v>
       </c>
       <c r="L110" t="s" s="2">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="M110" t="s" s="2">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="N110" s="2"/>
       <c r="O110" t="s" s="2">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="P110" t="s" s="2">
         <v>20</v>
@@ -14939,7 +14943,7 @@
         <v>20</v>
       </c>
       <c r="AF110" t="s" s="2">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="AG110" t="s" s="2">
         <v>75</v>
@@ -14957,21 +14961,21 @@
         <v>20</v>
       </c>
       <c r="AL110" t="s" s="2">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="AM110" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN110" t="s" s="2">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s" s="2">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="B111" t="s" s="2">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C111" s="2"/>
       <c r="D111" t="s" s="2">
@@ -14994,19 +14998,19 @@
         <v>85</v>
       </c>
       <c r="K111" t="s" s="2">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="L111" t="s" s="2">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="M111" t="s" s="2">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="N111" t="s" s="2">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="O111" t="s" s="2">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="P111" t="s" s="2">
         <v>20</v>
@@ -15055,7 +15059,7 @@
         <v>20</v>
       </c>
       <c r="AF111" t="s" s="2">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="AG111" t="s" s="2">
         <v>75</v>
@@ -15073,21 +15077,21 @@
         <v>20</v>
       </c>
       <c r="AL111" t="s" s="2">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="AM111" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN111" t="s" s="2">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s" s="2">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="B112" t="s" s="2">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C112" s="2"/>
       <c r="D112" t="s" s="2">
@@ -15113,16 +15117,16 @@
         <v>232</v>
       </c>
       <c r="L112" t="s" s="2">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="M112" t="s" s="2">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="N112" t="s" s="2">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="O112" t="s" s="2">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="P112" t="s" s="2">
         <v>20</v>
@@ -15171,7 +15175,7 @@
         <v>20</v>
       </c>
       <c r="AF112" t="s" s="2">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="AG112" t="s" s="2">
         <v>75</v>
@@ -15189,21 +15193,21 @@
         <v>20</v>
       </c>
       <c r="AL112" t="s" s="2">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="AM112" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN112" t="s" s="2">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s" s="2">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="B113" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="C113" s="2"/>
       <c r="D113" t="s" s="2">
@@ -15229,10 +15233,10 @@
         <v>232</v>
       </c>
       <c r="L113" t="s" s="2">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="M113" t="s" s="2">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="N113" s="2"/>
       <c r="O113" s="2"/>
@@ -15283,7 +15287,7 @@
         <v>20</v>
       </c>
       <c r="AF113" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="AG113" t="s" s="2">
         <v>84</v>
@@ -15301,7 +15305,7 @@
         <v>20</v>
       </c>
       <c r="AL113" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="AM113" t="s" s="2">
         <v>20</v>
@@ -15312,16 +15316,16 @@
     </row>
     <row r="114">
       <c r="A114" t="s" s="2">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B114" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C114" t="s" s="2">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="D114" t="s" s="2">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="E114" s="2"/>
       <c r="F114" t="s" s="2">
@@ -15343,14 +15347,14 @@
         <v>440</v>
       </c>
       <c r="L114" t="s" s="2">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="M114" t="s" s="2">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="N114" s="2"/>
       <c r="O114" t="s" s="2">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="P114" t="s" s="2">
         <v>20</v>
@@ -15399,7 +15403,7 @@
         <v>20</v>
       </c>
       <c r="AF114" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="AG114" t="s" s="2">
         <v>75</v>
@@ -15417,7 +15421,7 @@
         <v>20</v>
       </c>
       <c r="AL114" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="AM114" t="s" s="2">
         <v>20</v>
@@ -15428,10 +15432,10 @@
     </row>
     <row r="115">
       <c r="A115" t="s" s="2">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="B115" t="s" s="2">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C115" s="2"/>
       <c r="D115" t="s" s="2">
@@ -15540,10 +15544,10 @@
     </row>
     <row r="116">
       <c r="A116" t="s" s="2">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="B116" t="s" s="2">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C116" s="2"/>
       <c r="D116" t="s" s="2">
@@ -15654,10 +15658,10 @@
     </row>
     <row r="117">
       <c r="A117" t="s" s="2">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="B117" t="s" s="2">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="C117" s="2"/>
       <c r="D117" t="s" s="2">
@@ -15770,14 +15774,14 @@
     </row>
     <row r="118">
       <c r="A118" t="s" s="2">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="B118" t="s" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C118" s="2"/>
       <c r="D118" t="s" s="2">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="E118" s="2"/>
       <c r="F118" t="s" s="2">
@@ -15799,16 +15803,16 @@
         <v>189</v>
       </c>
       <c r="L118" t="s" s="2">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="M118" t="s" s="2">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="N118" t="s" s="2">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="O118" t="s" s="2">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="P118" t="s" s="2">
         <v>20</v>
@@ -15837,7 +15841,7 @@
       </c>
       <c r="Y118" s="2"/>
       <c r="Z118" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="AA118" t="s" s="2">
         <v>20</v>
@@ -15855,7 +15859,7 @@
         <v>20</v>
       </c>
       <c r="AF118" t="s" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="AG118" t="s" s="2">
         <v>84</v>
@@ -15873,7 +15877,7 @@
         <v>20</v>
       </c>
       <c r="AL118" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="AM118" t="s" s="2">
         <v>20</v>
@@ -15884,10 +15888,10 @@
     </row>
     <row r="119">
       <c r="A119" t="s" s="2">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B119" t="s" s="2">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C119" s="2"/>
       <c r="D119" t="s" s="2">
@@ -15996,10 +16000,10 @@
     </row>
     <row r="120">
       <c r="A120" t="s" s="2">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="B120" t="s" s="2">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="C120" s="2"/>
       <c r="D120" t="s" s="2">
@@ -16110,10 +16114,10 @@
     </row>
     <row r="121">
       <c r="A121" t="s" s="2">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="B121" t="s" s="2">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C121" s="2"/>
       <c r="D121" t="s" s="2">
@@ -16136,19 +16140,19 @@
         <v>85</v>
       </c>
       <c r="K121" t="s" s="2">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="L121" t="s" s="2">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="M121" t="s" s="2">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="N121" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="O121" t="s" s="2">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="P121" t="s" s="2">
         <v>20</v>
@@ -16197,7 +16201,7 @@
         <v>20</v>
       </c>
       <c r="AF121" t="s" s="2">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="AG121" t="s" s="2">
         <v>75</v>
@@ -16215,21 +16219,21 @@
         <v>20</v>
       </c>
       <c r="AL121" t="s" s="2">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="AM121" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN121" t="s" s="2">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s" s="2">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="B122" t="s" s="2">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C122" s="2"/>
       <c r="D122" t="s" s="2">
@@ -16338,10 +16342,10 @@
     </row>
     <row r="123">
       <c r="A123" t="s" s="2">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B123" t="s" s="2">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C123" s="2"/>
       <c r="D123" t="s" s="2">
@@ -16452,10 +16456,10 @@
     </row>
     <row r="124">
       <c r="A124" t="s" s="2">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B124" t="s" s="2">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="C124" s="2"/>
       <c r="D124" t="s" s="2">
@@ -16481,23 +16485,23 @@
         <v>98</v>
       </c>
       <c r="L124" t="s" s="2">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="M124" t="s" s="2">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="N124" t="s" s="2">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="O124" t="s" s="2">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="P124" t="s" s="2">
         <v>20</v>
       </c>
       <c r="Q124" s="2"/>
       <c r="R124" t="s" s="2">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="S124" t="s" s="2">
         <v>20</v>
@@ -16539,7 +16543,7 @@
         <v>20</v>
       </c>
       <c r="AF124" t="s" s="2">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="AG124" t="s" s="2">
         <v>75</v>
@@ -16557,21 +16561,21 @@
         <v>20</v>
       </c>
       <c r="AL124" t="s" s="2">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="AM124" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN124" t="s" s="2">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s" s="2">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="B125" t="s" s="2">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="C125" s="2"/>
       <c r="D125" t="s" s="2">
@@ -16597,13 +16601,13 @@
         <v>232</v>
       </c>
       <c r="L125" t="s" s="2">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="M125" t="s" s="2">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N125" t="s" s="2">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="O125" s="2"/>
       <c r="P125" t="s" s="2">
@@ -16653,7 +16657,7 @@
         <v>20</v>
       </c>
       <c r="AF125" t="s" s="2">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="AG125" t="s" s="2">
         <v>75</v>
@@ -16671,21 +16675,21 @@
         <v>20</v>
       </c>
       <c r="AL125" t="s" s="2">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="AM125" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN125" t="s" s="2">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s" s="2">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B126" t="s" s="2">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C126" s="2"/>
       <c r="D126" t="s" s="2">
@@ -16711,21 +16715,21 @@
         <v>104</v>
       </c>
       <c r="L126" t="s" s="2">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="M126" t="s" s="2">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="N126" s="2"/>
       <c r="O126" t="s" s="2">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="P126" t="s" s="2">
         <v>20</v>
       </c>
       <c r="Q126" s="2"/>
       <c r="R126" t="s" s="2">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="S126" t="s" s="2">
         <v>20</v>
@@ -16767,7 +16771,7 @@
         <v>20</v>
       </c>
       <c r="AF126" t="s" s="2">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="AG126" t="s" s="2">
         <v>75</v>
@@ -16785,21 +16789,21 @@
         <v>20</v>
       </c>
       <c r="AL126" t="s" s="2">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="AM126" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN126" t="s" s="2">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="s" s="2">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="B127" t="s" s="2">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C127" s="2"/>
       <c r="D127" t="s" s="2">
@@ -16825,14 +16829,14 @@
         <v>232</v>
       </c>
       <c r="L127" t="s" s="2">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="M127" t="s" s="2">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="N127" s="2"/>
       <c r="O127" t="s" s="2">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="P127" t="s" s="2">
         <v>20</v>
@@ -16881,7 +16885,7 @@
         <v>20</v>
       </c>
       <c r="AF127" t="s" s="2">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="AG127" t="s" s="2">
         <v>75</v>
@@ -16899,21 +16903,21 @@
         <v>20</v>
       </c>
       <c r="AL127" t="s" s="2">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="AM127" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN127" t="s" s="2">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="s" s="2">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="B128" t="s" s="2">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C128" s="2"/>
       <c r="D128" t="s" s="2">
@@ -16936,19 +16940,19 @@
         <v>85</v>
       </c>
       <c r="K128" t="s" s="2">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="L128" t="s" s="2">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="M128" t="s" s="2">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="N128" t="s" s="2">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="O128" t="s" s="2">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="P128" t="s" s="2">
         <v>20</v>
@@ -16997,7 +17001,7 @@
         <v>20</v>
       </c>
       <c r="AF128" t="s" s="2">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="AG128" t="s" s="2">
         <v>75</v>
@@ -17015,21 +17019,21 @@
         <v>20</v>
       </c>
       <c r="AL128" t="s" s="2">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="AM128" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN128" t="s" s="2">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s" s="2">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B129" t="s" s="2">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C129" s="2"/>
       <c r="D129" t="s" s="2">
@@ -17055,16 +17059,16 @@
         <v>232</v>
       </c>
       <c r="L129" t="s" s="2">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="M129" t="s" s="2">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="N129" t="s" s="2">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="O129" t="s" s="2">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="P129" t="s" s="2">
         <v>20</v>
@@ -17113,7 +17117,7 @@
         <v>20</v>
       </c>
       <c r="AF129" t="s" s="2">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="AG129" t="s" s="2">
         <v>75</v>
@@ -17131,21 +17135,21 @@
         <v>20</v>
       </c>
       <c r="AL129" t="s" s="2">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="AM129" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN129" t="s" s="2">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="s" s="2">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B130" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="C130" s="2"/>
       <c r="D130" t="s" s="2">
@@ -17171,10 +17175,10 @@
         <v>232</v>
       </c>
       <c r="L130" t="s" s="2">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="M130" t="s" s="2">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="N130" s="2"/>
       <c r="O130" s="2"/>
@@ -17225,7 +17229,7 @@
         <v>20</v>
       </c>
       <c r="AF130" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="AG130" t="s" s="2">
         <v>84</v>
@@ -17243,7 +17247,7 @@
         <v>20</v>
       </c>
       <c r="AL130" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="AM130" t="s" s="2">
         <v>20</v>
@@ -17254,10 +17258,10 @@
     </row>
     <row r="131">
       <c r="A131" t="s" s="2">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="B131" t="s" s="2">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="C131" s="2"/>
       <c r="D131" t="s" s="2">
@@ -17283,14 +17287,14 @@
         <v>440</v>
       </c>
       <c r="L131" t="s" s="2">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="M131" t="s" s="2">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="N131" s="2"/>
       <c r="O131" t="s" s="2">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="P131" t="s" s="2">
         <v>20</v>
@@ -17327,17 +17331,17 @@
         <v>20</v>
       </c>
       <c r="AB131" t="s" s="2">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="AC131" s="2"/>
       <c r="AD131" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AE131" t="s" s="2">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="AF131" t="s" s="2">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="AG131" t="s" s="2">
         <v>75</v>
@@ -17355,7 +17359,7 @@
         <v>20</v>
       </c>
       <c r="AL131" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="AM131" t="s" s="2">
         <v>20</v>
@@ -17366,10 +17370,10 @@
     </row>
     <row r="132">
       <c r="A132" t="s" s="2">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B132" t="s" s="2">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="C132" s="2"/>
       <c r="D132" t="s" s="2">
@@ -17478,10 +17482,10 @@
     </row>
     <row r="133">
       <c r="A133" t="s" s="2">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B133" t="s" s="2">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="C133" s="2"/>
       <c r="D133" t="s" s="2">
@@ -17592,10 +17596,10 @@
     </row>
     <row r="134">
       <c r="A134" t="s" s="2">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="B134" t="s" s="2">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="C134" s="2"/>
       <c r="D134" t="s" s="2">
@@ -17708,14 +17712,14 @@
     </row>
     <row r="135">
       <c r="A135" t="s" s="2">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="B135" t="s" s="2">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="C135" s="2"/>
       <c r="D135" t="s" s="2">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="E135" s="2"/>
       <c r="F135" t="s" s="2">
@@ -17737,14 +17741,14 @@
         <v>189</v>
       </c>
       <c r="L135" t="s" s="2">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="M135" t="s" s="2">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="N135" s="2"/>
       <c r="O135" t="s" s="2">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="P135" t="s" s="2">
         <v>20</v>
@@ -17772,7 +17776,7 @@
         <v>193</v>
       </c>
       <c r="Y135" t="s" s="2">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="Z135" t="s" s="2">
         <v>20</v>
@@ -17793,7 +17797,7 @@
         <v>20</v>
       </c>
       <c r="AF135" t="s" s="2">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="AG135" t="s" s="2">
         <v>84</v>
@@ -17811,7 +17815,7 @@
         <v>20</v>
       </c>
       <c r="AL135" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="AM135" t="s" s="2">
         <v>20</v>
@@ -17822,10 +17826,10 @@
     </row>
     <row r="136">
       <c r="A136" t="s" s="2">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="B136" t="s" s="2">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="C136" s="2"/>
       <c r="D136" t="s" s="2">
@@ -17848,17 +17852,17 @@
         <v>20</v>
       </c>
       <c r="K136" t="s" s="2">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="L136" t="s" s="2">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="M136" t="s" s="2">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="N136" s="2"/>
       <c r="O136" t="s" s="2">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="P136" t="s" s="2">
         <v>20</v>
@@ -17907,7 +17911,7 @@
         <v>20</v>
       </c>
       <c r="AF136" t="s" s="2">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="AG136" t="s" s="2">
         <v>84</v>
@@ -17925,7 +17929,7 @@
         <v>20</v>
       </c>
       <c r="AL136" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="AM136" t="s" s="2">
         <v>20</v>
@@ -17936,13 +17940,13 @@
     </row>
     <row r="137">
       <c r="A137" t="s" s="2">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B137" t="s" s="2">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="C137" t="s" s="2">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="D137" t="s" s="2">
         <v>20</v>
@@ -17967,14 +17971,14 @@
         <v>440</v>
       </c>
       <c r="L137" t="s" s="2">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="M137" t="s" s="2">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="N137" s="2"/>
       <c r="O137" t="s" s="2">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="P137" t="s" s="2">
         <v>20</v>
@@ -18023,7 +18027,7 @@
         <v>20</v>
       </c>
       <c r="AF137" t="s" s="2">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="AG137" t="s" s="2">
         <v>75</v>
@@ -18041,7 +18045,7 @@
         <v>20</v>
       </c>
       <c r="AL137" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="AM137" t="s" s="2">
         <v>20</v>
@@ -18052,10 +18056,10 @@
     </row>
     <row r="138">
       <c r="A138" t="s" s="2">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="B138" t="s" s="2">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="C138" s="2"/>
       <c r="D138" t="s" s="2">
@@ -18164,10 +18168,10 @@
     </row>
     <row r="139">
       <c r="A139" t="s" s="2">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="B139" t="s" s="2">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="C139" s="2"/>
       <c r="D139" t="s" s="2">
@@ -18278,10 +18282,10 @@
     </row>
     <row r="140">
       <c r="A140" t="s" s="2">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="B140" t="s" s="2">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="C140" s="2"/>
       <c r="D140" t="s" s="2">
@@ -18394,14 +18398,14 @@
     </row>
     <row r="141">
       <c r="A141" t="s" s="2">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="B141" t="s" s="2">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="C141" s="2"/>
       <c r="D141" t="s" s="2">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="E141" s="2"/>
       <c r="F141" t="s" s="2">
@@ -18423,14 +18427,14 @@
         <v>189</v>
       </c>
       <c r="L141" t="s" s="2">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="M141" t="s" s="2">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="N141" s="2"/>
       <c r="O141" t="s" s="2">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="P141" t="s" s="2">
         <v>20</v>
@@ -18459,7 +18463,7 @@
       </c>
       <c r="Y141" s="2"/>
       <c r="Z141" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="AA141" t="s" s="2">
         <v>20</v>
@@ -18477,7 +18481,7 @@
         <v>20</v>
       </c>
       <c r="AF141" t="s" s="2">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="AG141" t="s" s="2">
         <v>84</v>
@@ -18495,7 +18499,7 @@
         <v>20</v>
       </c>
       <c r="AL141" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="AM141" t="s" s="2">
         <v>20</v>
@@ -18506,10 +18510,10 @@
     </row>
     <row r="142">
       <c r="A142" t="s" s="2">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B142" t="s" s="2">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="C142" s="2"/>
       <c r="D142" t="s" s="2">
@@ -18618,10 +18622,10 @@
     </row>
     <row r="143">
       <c r="A143" t="s" s="2">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="B143" t="s" s="2">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="C143" s="2"/>
       <c r="D143" t="s" s="2">
@@ -18732,10 +18736,10 @@
     </row>
     <row r="144">
       <c r="A144" t="s" s="2">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="B144" t="s" s="2">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="C144" s="2"/>
       <c r="D144" t="s" s="2">
@@ -18758,19 +18762,19 @@
         <v>85</v>
       </c>
       <c r="K144" t="s" s="2">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="L144" t="s" s="2">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="M144" t="s" s="2">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="N144" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="O144" t="s" s="2">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="P144" t="s" s="2">
         <v>20</v>
@@ -18819,7 +18823,7 @@
         <v>20</v>
       </c>
       <c r="AF144" t="s" s="2">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="AG144" t="s" s="2">
         <v>75</v>
@@ -18837,21 +18841,21 @@
         <v>20</v>
       </c>
       <c r="AL144" t="s" s="2">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="AM144" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN144" t="s" s="2">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="s" s="2">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="B145" t="s" s="2">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="C145" s="2"/>
       <c r="D145" t="s" s="2">
@@ -18960,10 +18964,10 @@
     </row>
     <row r="146">
       <c r="A146" t="s" s="2">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="B146" t="s" s="2">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="C146" s="2"/>
       <c r="D146" t="s" s="2">
@@ -19074,10 +19078,10 @@
     </row>
     <row r="147">
       <c r="A147" t="s" s="2">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="B147" t="s" s="2">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="C147" s="2"/>
       <c r="D147" t="s" s="2">
@@ -19103,23 +19107,23 @@
         <v>98</v>
       </c>
       <c r="L147" t="s" s="2">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="M147" t="s" s="2">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="N147" t="s" s="2">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="O147" t="s" s="2">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="P147" t="s" s="2">
         <v>20</v>
       </c>
       <c r="Q147" s="2"/>
       <c r="R147" t="s" s="2">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="S147" t="s" s="2">
         <v>20</v>
@@ -19161,7 +19165,7 @@
         <v>20</v>
       </c>
       <c r="AF147" t="s" s="2">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="AG147" t="s" s="2">
         <v>75</v>
@@ -19179,21 +19183,21 @@
         <v>20</v>
       </c>
       <c r="AL147" t="s" s="2">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="AM147" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN147" t="s" s="2">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="s" s="2">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="B148" t="s" s="2">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="C148" s="2"/>
       <c r="D148" t="s" s="2">
@@ -19219,13 +19223,13 @@
         <v>232</v>
       </c>
       <c r="L148" t="s" s="2">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="M148" t="s" s="2">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N148" t="s" s="2">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="O148" s="2"/>
       <c r="P148" t="s" s="2">
@@ -19275,7 +19279,7 @@
         <v>20</v>
       </c>
       <c r="AF148" t="s" s="2">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="AG148" t="s" s="2">
         <v>75</v>
@@ -19293,21 +19297,21 @@
         <v>20</v>
       </c>
       <c r="AL148" t="s" s="2">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="AM148" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN148" t="s" s="2">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="s" s="2">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B149" t="s" s="2">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="C149" s="2"/>
       <c r="D149" t="s" s="2">
@@ -19333,21 +19337,21 @@
         <v>104</v>
       </c>
       <c r="L149" t="s" s="2">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="M149" t="s" s="2">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="N149" s="2"/>
       <c r="O149" t="s" s="2">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="P149" t="s" s="2">
         <v>20</v>
       </c>
       <c r="Q149" s="2"/>
       <c r="R149" t="s" s="2">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="S149" t="s" s="2">
         <v>20</v>
@@ -19389,7 +19393,7 @@
         <v>20</v>
       </c>
       <c r="AF149" t="s" s="2">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="AG149" t="s" s="2">
         <v>75</v>
@@ -19407,21 +19411,21 @@
         <v>20</v>
       </c>
       <c r="AL149" t="s" s="2">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="AM149" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN149" t="s" s="2">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="s" s="2">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="B150" t="s" s="2">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="C150" s="2"/>
       <c r="D150" t="s" s="2">
@@ -19447,14 +19451,14 @@
         <v>232</v>
       </c>
       <c r="L150" t="s" s="2">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="M150" t="s" s="2">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="N150" s="2"/>
       <c r="O150" t="s" s="2">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="P150" t="s" s="2">
         <v>20</v>
@@ -19503,7 +19507,7 @@
         <v>20</v>
       </c>
       <c r="AF150" t="s" s="2">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="AG150" t="s" s="2">
         <v>75</v>
@@ -19521,21 +19525,21 @@
         <v>20</v>
       </c>
       <c r="AL150" t="s" s="2">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="AM150" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN150" t="s" s="2">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="s" s="2">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B151" t="s" s="2">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="C151" s="2"/>
       <c r="D151" t="s" s="2">
@@ -19558,19 +19562,19 @@
         <v>85</v>
       </c>
       <c r="K151" t="s" s="2">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="L151" t="s" s="2">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="M151" t="s" s="2">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="N151" t="s" s="2">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="O151" t="s" s="2">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="P151" t="s" s="2">
         <v>20</v>
@@ -19619,7 +19623,7 @@
         <v>20</v>
       </c>
       <c r="AF151" t="s" s="2">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="AG151" t="s" s="2">
         <v>75</v>
@@ -19637,21 +19641,21 @@
         <v>20</v>
       </c>
       <c r="AL151" t="s" s="2">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="AM151" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN151" t="s" s="2">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="s" s="2">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="B152" t="s" s="2">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="C152" s="2"/>
       <c r="D152" t="s" s="2">
@@ -19677,16 +19681,16 @@
         <v>232</v>
       </c>
       <c r="L152" t="s" s="2">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="M152" t="s" s="2">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="N152" t="s" s="2">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="O152" t="s" s="2">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="P152" t="s" s="2">
         <v>20</v>
@@ -19735,7 +19739,7 @@
         <v>20</v>
       </c>
       <c r="AF152" t="s" s="2">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="AG152" t="s" s="2">
         <v>75</v>
@@ -19753,21 +19757,21 @@
         <v>20</v>
       </c>
       <c r="AL152" t="s" s="2">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="AM152" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN152" t="s" s="2">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="s" s="2">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="B153" t="s" s="2">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="C153" s="2"/>
       <c r="D153" t="s" s="2">
@@ -19793,14 +19797,14 @@
         <v>232</v>
       </c>
       <c r="L153" t="s" s="2">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="M153" t="s" s="2">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="N153" s="2"/>
       <c r="O153" t="s" s="2">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="P153" t="s" s="2">
         <v>20</v>
@@ -19849,7 +19853,7 @@
         <v>20</v>
       </c>
       <c r="AF153" t="s" s="2">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="AG153" t="s" s="2">
         <v>84</v>
@@ -19867,7 +19871,7 @@
         <v>20</v>
       </c>
       <c r="AL153" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="AM153" t="s" s="2">
         <v>20</v>

</xml_diff>